<commit_message>
Ajout du CRUD dans todo.controller.js
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_NomPrénom_Model.xlsx
+++ b/Journal-de-Travail_NomPrénom_Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Desktop\Projet_mongoDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Documents\GitHub\P_mongoDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBCF58B-5FA9-4741-A68B-DB9CACA4DD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B058E1-FCB8-42BC-8551-9842C3707480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Auteur:</t>
   </si>
@@ -170,6 +170,15 @@
   </si>
   <si>
     <t>finition des pools avec mongoose + model fini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustement des models </t>
+  </si>
+  <si>
+    <t>changement de mysql a mongo db pour la création de todos</t>
+  </si>
+  <si>
+    <t>CRUD de Todos avec mongoose dans le backend</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1185,7 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>245</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2106,16 +2115,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.20895522388059701</c:v>
+                  <c:v>0.13592233009708737</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73134328358208955</c:v>
+                  <c:v>0.82524271844660191</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9701492537313432E-2</c:v>
+                  <c:v>3.8834951456310676E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4304,7 +4313,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4359,7 +4368,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>5 heures 35 minutes</v>
+        <v>8 heures 35 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4374,15 +4383,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>335</v>
+        <v>455</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>335</v>
+        <v>515</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4706,45 +4715,71 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="str">
+      <c r="A18" s="62">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="30"/>
+        <v>19</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45782</v>
+      </c>
       <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
+      <c r="D18" s="32">
+        <v>45</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="G18" s="39"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="str">
+      <c r="A19" s="63">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="34"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="34">
+        <v>45782</v>
+      </c>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>45</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="62" t="str">
+      <c r="A20" s="62">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="30">
+        <v>45782</v>
+      </c>
+      <c r="C20" s="31">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>30</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -11050,7 +11085,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.20895522388059701</v>
+        <v>0.13592233009708737</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11067,15 +11102,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>245</v>
+        <v>365</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>245</v>
+        <v>425</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11083,11 +11118,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 05 min</v>
+        <v>7 h 05 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.73134328358208955</v>
+        <v>0.82524271844660191</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11161,7 +11196,7 @@
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>5.9701492537313432E-2</v>
+        <v>3.8834951456310676E-2</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11213,26 +11248,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>335</v>
+        <v>455</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>335</v>
+        <v>515</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>5 h 35 min</v>
+        <v>8 h 35 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>6.3446969696969696E-2</v>
+        <v>9.7537878787878785E-2</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11276,26 +11311,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11496,10 +11511,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11518,20 +11564,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>